<commit_message>
Foi implementado a edição selecionável na lista RDMARCAS, está funcionando corretamente
</commit_message>
<xml_diff>
--- a/storage/lista_calc_RDMarcas.xlsx
+++ b/storage/lista_calc_RDMarcas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,18 +447,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10050</v>
+        <v>1000</v>
       </c>
       <c r="B3" t="n">
-        <v>9950</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4">
@@ -482,7 +482,7 @@
         <v>2000</v>
       </c>
       <c r="B6" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7">
@@ -490,31 +490,15 @@
         <v>2000</v>
       </c>
       <c r="B7" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="B8" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B10" t="n">
-        <v>5000</v>
+        <v>1400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Foi adicionado o popup de consulta com rolagem de tamanho, porém as colunas não ficam alinhadas ainda.
</commit_message>
<xml_diff>
--- a/storage/lista_calc_RDMarcas.xlsx
+++ b/storage/lista_calc_RDMarcas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,14 +494,182 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B12" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B17" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B19" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B23" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B25" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B27" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B28" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>5000.0</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>5000.0</t>
         </is>
       </c>
     </row>

</xml_diff>